<commit_message>
pushing create patient without validations
</commit_message>
<xml_diff>
--- a/TesdData/Wonder_Dietician.xlsx
+++ b/TesdData/Wonder_Dietician.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harii\api-creepers\api_creepers\Wonder_Dietician\TesdData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C289589A-FD26-4FE1-8985-48C6BA3D4487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F91A64-05A8-46FA-A9D3-12EDD1CEAA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B94D65CF-50FC-4545-BBCA-65BB59FE26AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B94D65CF-50FC-4545-BBCA-65BB59FE26AB}"/>
   </bookViews>
   <sheets>
     <sheet name="userToken" sheetId="1" r:id="rId1"/>
+    <sheet name="createPatient" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Funny09</t>
   </si>
@@ -52,13 +53,31 @@
   </si>
   <si>
     <t>sumi_wonderdietician@gmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Allergy</t>
+  </si>
+  <si>
+    <t>FoodCategory</t>
+  </si>
+  <si>
+    <t>wonderdieticians@gmail.com</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
+  </si>
+  <si>
+    <t>Vegetarian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +89,19 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,9 +128,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142A6FC7-21DC-44C4-983C-A31C1761F5B5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -456,4 +490,48 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93386D0-EBC8-4B08-BFB4-EB04E43A1726}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{97E5E767-2E90-4201-A26A-750CF2017D4E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pushing sindu's changes directly to master
</commit_message>
<xml_diff>
--- a/TesdData/Wonder_Dietician.xlsx
+++ b/TesdData/Wonder_Dietician.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harii\api-creepers\api_creepers\Wonder_Dietician\TesdData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F91A64-05A8-46FA-A9D3-12EDD1CEAA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96906B95-3D5D-4F0D-BFC2-F55F29CD1D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B94D65CF-50FC-4545-BBCA-65BB59FE26AB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B94D65CF-50FC-4545-BBCA-65BB59FE26AB}"/>
   </bookViews>
   <sheets>
     <sheet name="userToken" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>userLoginEmail</t>
   </si>
   <si>
-    <t>sumi_wonderdietician@gmail.com</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>sam_wonderDietician@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142A6FC7-21DC-44C4-983C-A31C1761F5B5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -481,7 +481,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -496,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93386D0-EBC8-4B08-BFB4-EB04E43A1726}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -508,24 +508,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>